<commit_message>
Se agrega al Bloque 12(inventario_productos) un RotatingFileHandler
</commit_message>
<xml_diff>
--- a/Semana 1/inventario_producto.xlsx
+++ b/Semana 1/inventario_producto.xlsx
@@ -449,17 +449,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jamon</t>
+          <t>Jamonada</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>45</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>

</xml_diff>